<commit_message>
Just some prettying up of the com budget
</commit_message>
<xml_diff>
--- a/CMQA/Budgets/RCL-B-COM1.xlsx
+++ b/CMQA/Budgets/RCL-B-COM1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="420" yWindow="-15" windowWidth="8070" windowHeight="12000" activeTab="2"/>
+    <workbookView xWindow="420" yWindow="-15" windowWidth="8070" windowHeight="12000" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Intro" sheetId="4" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="51">
   <si>
     <t>Uplink Frequency</t>
   </si>
@@ -189,15 +189,97 @@
   <si>
     <t>UHF Downlink Data Rate</t>
   </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <r>
+      <t>m</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">2 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>kg s</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">-2 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>K</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-1</t>
+    </r>
+  </si>
+  <si>
+    <t>m/s</t>
+  </si>
+  <si>
+    <t>bps</t>
+  </si>
+  <si>
+    <t>UHF Uplink</t>
+  </si>
+  <si>
+    <t>UHF Downlink</t>
+  </si>
+  <si>
+    <t>Given</t>
+  </si>
+  <si>
+    <t>S-Band Uplink</t>
+  </si>
+  <si>
+    <t>S-Band Downlink</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -222,6 +304,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -231,7 +321,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="33">
+  <borders count="34">
     <border>
       <left/>
       <right/>
@@ -621,11 +711,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -665,59 +768,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -732,43 +790,96 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1071,10 +1182,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K29" sqref="K29:K30"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1082,99 +1193,123 @@
     <col min="1" max="1" width="25.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="63" t="s">
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="64" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="65" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="66">
         <v>6378135</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" s="61" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="62">
         <f>1.38065E-23</f>
         <v>1.38065E-23</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" s="63" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>40</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="62">
         <v>299790000</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" s="63" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="62">
         <v>300000</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" s="60" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>41</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="62">
         <f>100*1000</f>
         <v>100000</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" s="63" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="62">
         <v>1000000</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" s="63" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="62">
         <v>4000</v>
+      </c>
+      <c r="D8" s="63" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A1:D1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1182,8 +1317,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1192,25 +1327,25 @@
     <col min="2" max="2" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="18"/>
-      <c r="B1" s="59" t="s">
+      <c r="B1" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="59" t="s">
+      <c r="C1" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="60" t="s">
+      <c r="D1" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="61" t="s">
+      <c r="E1" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="62"/>
+      <c r="F1" s="57"/>
       <c r="G1" s="12"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1220,12 +1355,16 @@
       <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="27">
+      <c r="C2" s="40">
         <v>0.44</v>
       </c>
-      <c r="D2" s="27"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="50"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="F2" s="33" t="s">
+        <v>48</v>
+      </c>
       <c r="G2" s="12"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1233,10 +1372,10 @@
         <v>14</v>
       </c>
       <c r="B3" s="3"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="26"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="50"/>
       <c r="E3" s="7"/>
-      <c r="F3" s="53"/>
+      <c r="F3" s="35"/>
       <c r="G3" s="8"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1246,12 +1385,12 @@
       <c r="B4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="27">
+      <c r="C4" s="40">
         <v>100</v>
       </c>
-      <c r="D4" s="27"/>
+      <c r="D4" s="40"/>
       <c r="E4" s="6"/>
-      <c r="F4" s="54"/>
+      <c r="F4" s="36"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
@@ -1260,10 +1399,10 @@
       <c r="B5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="27">
+      <c r="C5" s="40">
         <v>30</v>
       </c>
-      <c r="D5" s="27"/>
+      <c r="D5" s="40"/>
       <c r="E5" s="7"/>
       <c r="F5" s="22"/>
       <c r="G5" s="12"/>
@@ -1275,28 +1414,28 @@
       <c r="B6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="27">
+      <c r="C6" s="40">
         <v>2</v>
       </c>
-      <c r="D6" s="27"/>
+      <c r="D6" s="40"/>
       <c r="E6" s="7"/>
       <c r="F6" s="8"/>
       <c r="G6" s="12"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="33" t="s">
+      <c r="A7" s="26" t="s">
         <v>10</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="37">
+      <c r="C7" s="55">
         <f>10*LOG(C4)</f>
         <v>20</v>
       </c>
-      <c r="D7" s="37"/>
+      <c r="D7" s="55"/>
       <c r="E7" s="6"/>
-      <c r="F7" s="54"/>
+      <c r="F7" s="36"/>
       <c r="G7" s="12"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1306,43 +1445,43 @@
       <c r="B8" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="48">
+      <c r="C8" s="45">
         <f>290*(10^(C6/10)-1)</f>
         <v>169.61902581372294</v>
       </c>
-      <c r="D8" s="48"/>
+      <c r="D8" s="45"/>
       <c r="E8" s="4"/>
       <c r="F8" s="14"/>
       <c r="G8" s="12"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="33" t="s">
+      <c r="A9" s="26" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="49">
+      <c r="C9" s="46">
         <f>C5-10*LOG(C8)</f>
         <v>7.7052543543729222</v>
       </c>
-      <c r="D9" s="49"/>
+      <c r="D9" s="46"/>
       <c r="E9" s="7"/>
-      <c r="F9" s="54"/>
+      <c r="F9" s="36"/>
       <c r="G9" s="12"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="32" t="s">
+      <c r="A10" s="25" t="s">
         <v>11</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="29">
+      <c r="C10" s="23">
         <f>(radEarth*(((((alt+radEarth)^2)/(radEarth^2))-(COS(0))^2)^(1/2)-SIN(0)))/1000</f>
         <v>1979.1111641340412</v>
       </c>
-      <c r="D10" s="29">
+      <c r="D10" s="23">
         <f>(radEarth*(((((alt+radEarth)^2)/(radEarth^2))-(COS(RADIANS(90)))^2)^(1/2)-SIN(RADIANS(90))))/1000</f>
         <v>300.00000000000011</v>
       </c>
@@ -1351,68 +1490,68 @@
       <c r="G10" s="12"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="33" t="s">
+      <c r="A11" s="26" t="s">
         <v>27</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="30">
+      <c r="C11" s="24">
         <f>20*LOG((C10*1000))</f>
         <v>125.92940377310335</v>
       </c>
-      <c r="D11" s="30">
+      <c r="D11" s="24">
         <f>20*LOG((D10*1000))</f>
         <v>109.54242509439325</v>
       </c>
       <c r="E11" s="7"/>
-      <c r="F11" s="54"/>
+      <c r="F11" s="36"/>
       <c r="G11" s="12"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="33" t="s">
+      <c r="A12" s="26" t="s">
         <v>28</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="48">
+      <c r="C12" s="45">
         <f>10*LOG(ul)</f>
         <v>36.020599913279625</v>
       </c>
-      <c r="D12" s="48"/>
+      <c r="D12" s="45"/>
       <c r="E12" s="7"/>
       <c r="F12" s="13"/>
       <c r="G12" s="12"/>
     </row>
     <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="33" t="s">
+      <c r="A13" s="26" t="s">
         <v>33</v>
       </c>
       <c r="B13" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="38">
+      <c r="C13" s="43">
         <f>20*LOG(4*PI()/c_)+10*LOG(k)</f>
         <v>-376.15130958980478</v>
       </c>
-      <c r="D13" s="39"/>
+      <c r="D13" s="44"/>
       <c r="E13" s="7"/>
       <c r="F13" s="13"/>
       <c r="G13" s="12"/>
     </row>
     <row r="14" spans="1:7" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="44" t="s">
+      <c r="A14" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="45" t="s">
+      <c r="B14" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="46">
+      <c r="C14" s="31">
         <f>C7+C9-C13-C11-(20*LOG(C2*10^9))-C12</f>
         <v>69.03750672807098</v>
       </c>
-      <c r="D14" s="46">
+      <c r="D14" s="31">
         <f>C7+C9-C13-D11-(20*LOG(C2*10^9))-C12</f>
         <v>85.424485406781059</v>
       </c>
@@ -1427,12 +1566,16 @@
       <c r="B15" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="23">
+      <c r="C15" s="53">
         <v>0.44</v>
       </c>
-      <c r="D15" s="24"/>
-      <c r="E15" s="58"/>
-      <c r="F15" s="16"/>
+      <c r="D15" s="54"/>
+      <c r="E15" s="37" t="s">
+        <v>47</v>
+      </c>
+      <c r="F15" s="67" t="s">
+        <v>48</v>
+      </c>
       <c r="G15" s="12"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -1440,10 +1583,10 @@
         <v>14</v>
       </c>
       <c r="B16" s="3"/>
-      <c r="C16" s="25" t="s">
+      <c r="C16" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="26"/>
+      <c r="D16" s="50"/>
       <c r="E16" s="4"/>
       <c r="F16" s="14"/>
     </row>
@@ -1454,12 +1597,14 @@
       <c r="B17" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="25">
+      <c r="C17" s="49">
         <v>5</v>
       </c>
-      <c r="D17" s="26"/>
+      <c r="D17" s="50"/>
       <c r="E17" s="7"/>
-      <c r="F17" s="8"/>
+      <c r="F17" s="33" t="s">
+        <v>48</v>
+      </c>
       <c r="G17" s="12"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -1469,12 +1614,14 @@
       <c r="B18" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="34">
+      <c r="C18" s="47">
         <v>5</v>
       </c>
-      <c r="D18" s="35"/>
+      <c r="D18" s="48"/>
       <c r="E18" s="7"/>
-      <c r="F18" s="13"/>
+      <c r="F18" s="35" t="s">
+        <v>48</v>
+      </c>
       <c r="K18" s="8"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -1484,28 +1631,28 @@
       <c r="B19" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="27">
+      <c r="C19" s="40">
         <v>2</v>
       </c>
-      <c r="D19" s="27"/>
+      <c r="D19" s="40"/>
       <c r="E19" s="4"/>
       <c r="F19" s="8"/>
       <c r="G19" s="12"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="33" t="s">
+      <c r="A20" s="26" t="s">
         <v>10</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C20" s="40">
+      <c r="C20" s="51">
         <f>10*LOG(C17)</f>
         <v>6.9897000433601884</v>
       </c>
-      <c r="D20" s="41"/>
+      <c r="D20" s="52"/>
       <c r="E20" s="7"/>
-      <c r="F20" s="54"/>
+      <c r="F20" s="36"/>
       <c r="G20" s="12"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -1515,43 +1662,43 @@
       <c r="B21" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C21" s="48">
+      <c r="C21" s="45">
         <f>290*(10^(C19/10)-1)</f>
         <v>169.61902581372294</v>
       </c>
-      <c r="D21" s="48"/>
+      <c r="D21" s="45"/>
       <c r="E21" s="4"/>
       <c r="F21" s="14"/>
       <c r="G21" s="12"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="33" t="s">
+      <c r="A22" s="26" t="s">
         <v>15</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="31">
+      <c r="C22" s="41">
         <f>C18-(10*LOG(C21))</f>
         <v>-17.294745645627078</v>
       </c>
-      <c r="D22" s="36"/>
+      <c r="D22" s="42"/>
       <c r="E22" s="6"/>
-      <c r="F22" s="54"/>
+      <c r="F22" s="36"/>
       <c r="G22" s="12"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="32" t="s">
+      <c r="A23" s="25" t="s">
         <v>11</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C23" s="29">
+      <c r="C23" s="23">
         <f>(radEarth*(((((alt+radEarth)^2)/(radEarth^2))-(COS(0))^2)^(1/2)-SIN(0)))/1000</f>
         <v>1979.1111641340412</v>
       </c>
-      <c r="D23" s="29">
+      <c r="D23" s="23">
         <f>(radEarth*(((((alt+radEarth)^2)/(radEarth^2))-(COS(RADIANS(90)))^2)^(1/2)-SIN(RADIANS(90))))/1000</f>
         <v>300.00000000000011</v>
       </c>
@@ -1560,68 +1707,70 @@
       <c r="G23" s="12"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="33" t="s">
+      <c r="A24" s="26" t="s">
         <v>27</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="30">
+      <c r="C24" s="24">
         <f>20*LOG((C23*1000))</f>
         <v>125.92940377310335</v>
       </c>
-      <c r="D24" s="30">
+      <c r="D24" s="24">
         <f>20*LOG((D23*1000))</f>
         <v>109.54242509439325</v>
       </c>
       <c r="E24" s="6"/>
-      <c r="F24" s="54"/>
+      <c r="F24" s="36"/>
       <c r="G24" s="12"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="33" t="s">
+      <c r="A25" s="26" t="s">
         <v>28</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C25" s="27">
+      <c r="C25" s="40">
         <f>10*LOG(udl)</f>
         <v>50</v>
       </c>
-      <c r="D25" s="27"/>
+      <c r="D25" s="40"/>
       <c r="E25" s="7"/>
-      <c r="F25" s="8"/>
+      <c r="F25" s="35" t="s">
+        <v>48</v>
+      </c>
       <c r="G25" s="12"/>
     </row>
     <row r="26" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="33" t="s">
+      <c r="A26" s="26" t="s">
         <v>33</v>
       </c>
       <c r="B26" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C26" s="38">
+      <c r="C26" s="43">
         <f>20*LOG(4*PI()/c_)+10*LOG(k)</f>
         <v>-376.15130958980478</v>
       </c>
-      <c r="D26" s="39"/>
+      <c r="D26" s="44"/>
       <c r="E26" s="7"/>
-      <c r="F26" s="8"/>
+      <c r="F26" s="35"/>
       <c r="G26" s="12"/>
     </row>
     <row r="27" spans="1:11" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="44" t="s">
+      <c r="A27" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="B27" s="45" t="s">
+      <c r="B27" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="C27" s="46">
+      <c r="C27" s="31">
         <f>C20+C22-C26-C24-(20*LOG(C15*10^9))-C25</f>
         <v>17.047806684710793</v>
       </c>
-      <c r="D27" s="47">
+      <c r="D27" s="32">
         <f>C20+C22-C26-D24-(20*LOG(C15*10^9))-C25</f>
         <v>33.434785363420872</v>
       </c>
@@ -1631,7 +1780,7 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="22"/>
-      <c r="B28" s="42"/>
+      <c r="B28" s="27"/>
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
       <c r="E28" s="16"/>
@@ -1640,7 +1789,7 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="22"/>
-      <c r="B29" s="42"/>
+      <c r="B29" s="27"/>
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
       <c r="E29" s="8"/>
@@ -1649,7 +1798,7 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="22"/>
-      <c r="B30" s="42"/>
+      <c r="B30" s="27"/>
       <c r="C30" s="8"/>
       <c r="D30" s="8"/>
       <c r="E30" s="8"/>
@@ -1657,7 +1806,7 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="22"/>
-      <c r="B31" s="42"/>
+      <c r="B31" s="27"/>
       <c r="C31" s="8"/>
       <c r="D31" s="8"/>
       <c r="E31" s="8"/>
@@ -1666,7 +1815,7 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="22"/>
-      <c r="B32" s="42"/>
+      <c r="B32" s="27"/>
       <c r="C32" s="8"/>
       <c r="D32" s="8"/>
       <c r="E32" s="8"/>
@@ -1674,16 +1823,16 @@
       <c r="G32" s="8"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="43"/>
-      <c r="B33" s="42"/>
+      <c r="A33" s="28"/>
+      <c r="B33" s="27"/>
       <c r="C33" s="8"/>
       <c r="D33" s="8"/>
       <c r="E33" s="8"/>
       <c r="F33" s="8"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="43"/>
-      <c r="B34" s="42"/>
+      <c r="A34" s="28"/>
+      <c r="B34" s="27"/>
       <c r="C34" s="8"/>
       <c r="D34" s="8"/>
       <c r="E34" s="8"/>
@@ -1692,7 +1841,7 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="22"/>
-      <c r="B35" s="42"/>
+      <c r="B35" s="27"/>
       <c r="C35" s="8"/>
       <c r="D35" s="8"/>
       <c r="E35" s="8"/>
@@ -1701,7 +1850,7 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="22"/>
-      <c r="B36" s="42"/>
+      <c r="B36" s="27"/>
       <c r="C36" s="8"/>
       <c r="D36" s="8"/>
       <c r="E36" s="8"/>
@@ -1709,8 +1858,8 @@
       <c r="G36" s="8"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="43"/>
-      <c r="B37" s="42"/>
+      <c r="A37" s="28"/>
+      <c r="B37" s="27"/>
       <c r="C37" s="8"/>
       <c r="D37" s="8"/>
       <c r="E37" s="8"/>
@@ -1719,7 +1868,7 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="22"/>
-      <c r="B38" s="42"/>
+      <c r="B38" s="27"/>
       <c r="C38" s="8"/>
       <c r="D38" s="8"/>
       <c r="E38" s="8"/>
@@ -1728,7 +1877,7 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="22"/>
-      <c r="B39" s="42"/>
+      <c r="B39" s="27"/>
       <c r="C39" s="8"/>
       <c r="D39" s="8"/>
       <c r="E39" s="8"/>
@@ -1736,8 +1885,8 @@
       <c r="G39" s="8"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="43"/>
-      <c r="B40" s="42"/>
+      <c r="A40" s="28"/>
+      <c r="B40" s="27"/>
       <c r="C40" s="8"/>
       <c r="D40" s="8"/>
       <c r="E40" s="8"/>
@@ -1750,6 +1899,15 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
     <mergeCell ref="C22:D22"/>
     <mergeCell ref="C25:D25"/>
     <mergeCell ref="C26:D26"/>
@@ -1762,15 +1920,6 @@
     <mergeCell ref="C20:D20"/>
     <mergeCell ref="C21:D21"/>
     <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="C12:D12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -1781,8 +1930,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1791,25 +1940,25 @@
     <col min="2" max="2" width="5.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="18"/>
-      <c r="B1" s="59" t="s">
+      <c r="B1" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="59" t="s">
+      <c r="C1" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="60" t="s">
+      <c r="D1" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="61" t="s">
+      <c r="E1" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="62"/>
+      <c r="F1" s="57"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
@@ -1818,12 +1967,16 @@
       <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="27">
+      <c r="C2" s="40">
         <v>2.4</v>
       </c>
-      <c r="D2" s="25"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="22"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" s="33" t="s">
+        <v>48</v>
+      </c>
       <c r="G2" s="12"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -1831,10 +1984,10 @@
         <v>14</v>
       </c>
       <c r="B3" s="3"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="56"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="52"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="58"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="35"/>
       <c r="G3" s="12"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -1844,12 +1997,12 @@
       <c r="B4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="27">
+      <c r="C4" s="40">
         <v>100</v>
       </c>
-      <c r="D4" s="27"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="54"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="36"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
@@ -1858,12 +2011,12 @@
       <c r="B5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="27">
+      <c r="C5" s="40">
         <v>30</v>
       </c>
-      <c r="D5" s="27"/>
+      <c r="D5" s="40"/>
       <c r="E5" s="7"/>
-      <c r="F5" s="53"/>
+      <c r="F5" s="35"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
@@ -1872,27 +2025,27 @@
       <c r="B6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="27">
+      <c r="C6" s="40">
         <v>2</v>
       </c>
-      <c r="D6" s="27"/>
+      <c r="D6" s="40"/>
       <c r="E6" s="7"/>
-      <c r="F6" s="13"/>
+      <c r="F6" s="14"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="33" t="s">
+      <c r="A7" s="26" t="s">
         <v>10</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="37">
+      <c r="C7" s="55">
         <f>10*LOG(C4)</f>
         <v>20</v>
       </c>
-      <c r="D7" s="37"/>
+      <c r="D7" s="55"/>
       <c r="E7" s="6"/>
-      <c r="F7" s="54"/>
+      <c r="F7" s="36"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
@@ -1901,112 +2054,114 @@
       <c r="B8" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="48">
+      <c r="C8" s="45">
         <f>290*(10^(C6/10)-1)</f>
         <v>169.61902581372294</v>
       </c>
-      <c r="D8" s="48"/>
-      <c r="E8" s="7"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="4"/>
       <c r="F8" s="14"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="33" t="s">
+      <c r="A9" s="26" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="49">
+      <c r="C9" s="46">
         <f>C5-10*LOG(C8)</f>
         <v>7.7052543543729222</v>
       </c>
-      <c r="D9" s="49"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="54"/>
+      <c r="D9" s="46"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="36"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="32" t="s">
+      <c r="A10" s="25" t="s">
         <v>11</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="29">
+      <c r="C10" s="23">
         <f>(radEarth*(((((alt+radEarth)^2)/(radEarth^2))-(COS(0))^2)^(1/2)-SIN(0)))/1000</f>
         <v>1979.1111641340412</v>
       </c>
-      <c r="D10" s="29">
+      <c r="D10" s="23">
         <f>(radEarth*(((((alt+radEarth)^2)/(radEarth^2))-(COS(RADIANS(90)))^2)^(1/2)-SIN(RADIANS(90))))/1000</f>
         <v>300.00000000000011</v>
       </c>
       <c r="E10" s="4"/>
-      <c r="F10" s="13"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="12"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="33" t="s">
+      <c r="A11" s="26" t="s">
         <v>27</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="30">
+      <c r="C11" s="24">
         <f>20*LOG((C10*1000))</f>
         <v>125.92940377310335</v>
       </c>
-      <c r="D11" s="30">
+      <c r="D11" s="24">
         <f>20*LOG((D10*1000))</f>
         <v>109.54242509439325</v>
       </c>
       <c r="E11" s="7"/>
-      <c r="F11" s="54"/>
+      <c r="F11" s="36"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="33" t="s">
+      <c r="A12" s="26" t="s">
         <v>28</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="48">
+      <c r="C12" s="45">
         <f>10*LOG(ul)</f>
         <v>36.020599913279625</v>
       </c>
-      <c r="D12" s="48"/>
+      <c r="D12" s="45"/>
       <c r="E12" s="7"/>
       <c r="F12" s="13"/>
     </row>
     <row r="13" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="33" t="s">
+      <c r="A13" s="26" t="s">
         <v>33</v>
       </c>
       <c r="B13" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="38">
+      <c r="C13" s="43">
         <f>20*LOG(4*PI()/c_)+10*LOG(k)</f>
         <v>-376.15130958980478</v>
       </c>
-      <c r="D13" s="39"/>
+      <c r="D13" s="44"/>
       <c r="E13" s="7"/>
       <c r="F13" s="13"/>
     </row>
     <row r="14" spans="1:12" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="44" t="s">
+      <c r="A14" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="45" t="s">
+      <c r="B14" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="46">
+      <c r="C14" s="31">
         <f>C7+C9-C13-C11-(20*LOG(C2*10^9))-C12</f>
         <v>54.302335423562624</v>
       </c>
-      <c r="D14" s="46">
+      <c r="D14" s="31">
         <f>C7+C9-C13-D11-(20*LOG(C2*10^9))-C12</f>
         <v>70.689314102272704</v>
       </c>
       <c r="E14" s="7"/>
-      <c r="F14" s="13"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="12"/>
       <c r="L14" s="8"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -2016,231 +2171,242 @@
       <c r="B15" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="23">
+      <c r="C15" s="53">
         <v>2.4</v>
       </c>
-      <c r="D15" s="55"/>
-      <c r="E15" s="58"/>
-      <c r="F15" s="57"/>
+      <c r="D15" s="59"/>
+      <c r="E15" s="37" t="s">
+        <v>50</v>
+      </c>
+      <c r="F15" s="67" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
         <v>14</v>
       </c>
       <c r="B16" s="3"/>
-      <c r="C16" s="25" t="s">
+      <c r="C16" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="26"/>
-      <c r="E16" s="8"/>
+      <c r="D16" s="50"/>
+      <c r="E16" s="4"/>
       <c r="F16" s="14"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
         <v>18</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="25">
+      <c r="C17" s="49">
         <v>5</v>
       </c>
-      <c r="D17" s="26"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="13"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D17" s="50"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="33" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="17" t="s">
         <v>2</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="34">
+      <c r="C18" s="47">
         <v>5</v>
       </c>
-      <c r="D18" s="35"/>
+      <c r="D18" s="48"/>
       <c r="E18" s="7"/>
-      <c r="F18" s="13"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F18" s="35" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="17" t="s">
         <v>25</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="27">
+      <c r="C19" s="40">
         <v>2</v>
       </c>
-      <c r="D19" s="27"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="13"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="33" t="s">
+      <c r="D19" s="40"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="12"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="26" t="s">
         <v>10</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C20" s="40">
+      <c r="C20" s="51">
         <f>10*LOG(C17)</f>
         <v>6.9897000433601884</v>
       </c>
-      <c r="D20" s="41"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="54"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D20" s="52"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="36"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="17" t="s">
         <v>26</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C21" s="48">
+      <c r="C21" s="45">
         <f>290*(10^(C19/10)-1)</f>
         <v>169.61902581372294</v>
       </c>
-      <c r="D21" s="48"/>
-      <c r="E21" s="7"/>
+      <c r="D21" s="45"/>
+      <c r="E21" s="4"/>
       <c r="F21" s="14"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="33" t="s">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="26" t="s">
         <v>15</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="31">
+      <c r="C22" s="41">
         <f>C18-(10*LOG(C21))</f>
         <v>-17.294745645627078</v>
       </c>
-      <c r="D22" s="36"/>
+      <c r="D22" s="42"/>
       <c r="E22" s="6"/>
-      <c r="F22" s="54"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="32" t="s">
+      <c r="F22" s="36"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="25" t="s">
         <v>11</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C23" s="29">
+      <c r="C23" s="23">
         <f>(radEarth*(((((alt+radEarth)^2)/(radEarth^2))-(COS(0))^2)^(1/2)-SIN(0)))/1000</f>
         <v>1979.1111641340412</v>
       </c>
-      <c r="D23" s="29">
+      <c r="D23" s="23">
         <f>(radEarth*(((((alt+radEarth)^2)/(radEarth^2))-(COS(RADIANS(90)))^2)^(1/2)-SIN(RADIANS(90))))/1000</f>
         <v>300.00000000000011</v>
       </c>
       <c r="E23" s="4"/>
       <c r="F23" s="14"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="33" t="s">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="26" t="s">
         <v>27</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="30">
+      <c r="C24" s="24">
         <f>20*LOG((C23*1000))</f>
         <v>125.92940377310335</v>
       </c>
-      <c r="D24" s="30">
+      <c r="D24" s="24">
         <f>20*LOG((D23*1000))</f>
         <v>109.54242509439325</v>
       </c>
       <c r="E24" s="6"/>
-      <c r="F24" s="54"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="33" t="s">
+      <c r="F24" s="36"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="26" t="s">
         <v>28</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C25" s="27">
+      <c r="C25" s="40">
         <f>10*LOG(sdl)</f>
         <v>60</v>
       </c>
-      <c r="D25" s="27"/>
+      <c r="D25" s="40"/>
       <c r="E25" s="7"/>
-      <c r="F25" s="13"/>
-    </row>
-    <row r="26" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="33" t="s">
+      <c r="F25" s="35" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="26" t="s">
         <v>33</v>
       </c>
       <c r="B26" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C26" s="38">
+      <c r="C26" s="43">
         <f>20*LOG(4*PI()/c_)+10*LOG(k)</f>
         <v>-376.15130958980478</v>
       </c>
-      <c r="D26" s="39"/>
+      <c r="D26" s="44"/>
       <c r="E26" s="7"/>
-      <c r="F26" s="13"/>
-    </row>
-    <row r="27" spans="1:6" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="44" t="s">
+      <c r="F26" s="35"/>
+    </row>
+    <row r="27" spans="1:7" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A27" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="B27" s="45" t="s">
+      <c r="B27" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="C27" s="46">
+      <c r="C27" s="31">
         <f>C20+C22-C26-C24-(20*LOG(C15*10^9))-C25</f>
         <v>-7.6873646197975631</v>
       </c>
-      <c r="D27" s="47">
+      <c r="D27" s="32">
         <f>C20+C22-C26-D24-(20*LOG(C15*10^9))-C25</f>
         <v>8.6996140589125162</v>
       </c>
       <c r="E27" s="11"/>
       <c r="F27" s="15"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="22"/>
-      <c r="B28" s="42"/>
+      <c r="B28" s="27"/>
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
       <c r="E28" s="8"/>
       <c r="F28" s="8"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="22"/>
-      <c r="B29" s="42"/>
+      <c r="B29" s="27"/>
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
       <c r="E29" s="8"/>
       <c r="F29" s="8"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="22"/>
-      <c r="B30" s="42"/>
+      <c r="B30" s="27"/>
       <c r="C30" s="8"/>
       <c r="D30" s="8"/>
       <c r="E30" s="8"/>
       <c r="F30" s="8"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="22"/>
-      <c r="B31" s="42"/>
+      <c r="B31" s="27"/>
       <c r="C31" s="8"/>
       <c r="D31" s="8"/>
       <c r="E31" s="8"/>
       <c r="F31" s="8"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="51"/>
-      <c r="B32" s="42"/>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="34"/>
+      <c r="B32" s="27"/>
       <c r="C32" s="8"/>
       <c r="D32" s="8"/>
       <c r="E32" s="8"/>
@@ -2248,7 +2414,7 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="22"/>
-      <c r="B33" s="42"/>
+      <c r="B33" s="27"/>
       <c r="C33" s="8"/>
       <c r="D33" s="8"/>
       <c r="E33" s="8"/>
@@ -2256,7 +2422,7 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="22"/>
-      <c r="B34" s="42"/>
+      <c r="B34" s="27"/>
       <c r="C34" s="8"/>
       <c r="D34" s="8"/>
       <c r="E34" s="8"/>
@@ -2264,7 +2430,7 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="22"/>
-      <c r="B35" s="42"/>
+      <c r="B35" s="27"/>
       <c r="C35" s="8"/>
       <c r="D35" s="8"/>
       <c r="E35" s="8"/>
@@ -2272,7 +2438,7 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="22"/>
-      <c r="B36" s="42"/>
+      <c r="B36" s="27"/>
       <c r="C36" s="8"/>
       <c r="D36" s="8"/>
       <c r="E36" s="8"/>
@@ -2280,7 +2446,7 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="22"/>
-      <c r="B37" s="42"/>
+      <c r="B37" s="27"/>
       <c r="C37" s="8"/>
       <c r="D37" s="8"/>
       <c r="E37" s="8"/>
@@ -2288,7 +2454,7 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="22"/>
-      <c r="B38" s="42"/>
+      <c r="B38" s="27"/>
       <c r="C38" s="8"/>
       <c r="D38" s="8"/>
       <c r="E38" s="8"/>
@@ -2296,7 +2462,7 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="22"/>
-      <c r="B39" s="42"/>
+      <c r="B39" s="27"/>
       <c r="C39" s="8"/>
       <c r="D39" s="8"/>
       <c r="E39" s="8"/>
@@ -2304,7 +2470,7 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="22"/>
-      <c r="B40" s="42"/>
+      <c r="B40" s="27"/>
       <c r="C40" s="8"/>
       <c r="D40" s="8"/>
       <c r="E40" s="8"/>
@@ -2312,23 +2478,23 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="22"/>
-      <c r="B41" s="42"/>
+      <c r="B41" s="27"/>
       <c r="C41" s="8"/>
       <c r="D41" s="8"/>
       <c r="E41" s="8"/>
       <c r="F41" s="8"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="43"/>
-      <c r="B42" s="42"/>
+      <c r="A42" s="28"/>
+      <c r="B42" s="27"/>
       <c r="C42" s="8"/>
       <c r="D42" s="8"/>
       <c r="E42" s="8"/>
       <c r="F42" s="8"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="43"/>
-      <c r="B43" s="42"/>
+      <c r="A43" s="28"/>
+      <c r="B43" s="27"/>
       <c r="C43" s="8"/>
       <c r="D43" s="8"/>
       <c r="E43" s="8"/>
@@ -2336,7 +2502,7 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="22"/>
-      <c r="B44" s="42"/>
+      <c r="B44" s="27"/>
       <c r="C44" s="8"/>
       <c r="D44" s="8"/>
       <c r="E44" s="8"/>
@@ -2344,15 +2510,15 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="22"/>
-      <c r="B45" s="42"/>
+      <c r="B45" s="27"/>
       <c r="C45" s="8"/>
       <c r="D45" s="8"/>
       <c r="E45" s="8"/>
       <c r="F45" s="8"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="43"/>
-      <c r="B46" s="42"/>
+      <c r="A46" s="28"/>
+      <c r="B46" s="27"/>
       <c r="C46" s="8"/>
       <c r="D46" s="8"/>
       <c r="E46" s="8"/>
@@ -2360,7 +2526,7 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="22"/>
-      <c r="B47" s="42"/>
+      <c r="B47" s="27"/>
       <c r="C47" s="8"/>
       <c r="D47" s="8"/>
       <c r="E47" s="8"/>
@@ -2368,15 +2534,15 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="22"/>
-      <c r="B48" s="42"/>
+      <c r="B48" s="27"/>
       <c r="C48" s="8"/>
       <c r="D48" s="8"/>
       <c r="E48" s="8"/>
       <c r="F48" s="8"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="43"/>
-      <c r="B49" s="42"/>
+      <c r="A49" s="28"/>
+      <c r="B49" s="27"/>
       <c r="C49" s="8"/>
       <c r="D49" s="8"/>
       <c r="E49" s="8"/>
@@ -2387,12 +2553,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="C25:D25"/>
@@ -2408,6 +2568,12 @@
     <mergeCell ref="C15:D15"/>
     <mergeCell ref="C16:D16"/>
     <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
More precise speed of light
</commit_message>
<xml_diff>
--- a/CMQA/Budgets/RCL-B-COM1.xlsx
+++ b/CMQA/Budgets/RCL-B-COM1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="420" yWindow="-15" windowWidth="8070" windowHeight="12000" activeTab="1"/>
+    <workbookView xWindow="420" yWindow="-15" windowWidth="8070" windowHeight="12000"/>
   </bookViews>
   <sheets>
     <sheet name="Intro" sheetId="4" r:id="rId1"/>
@@ -251,9 +251,6 @@
     </r>
   </si>
   <si>
-    <t>m/s</t>
-  </si>
-  <si>
     <t>bps</t>
   </si>
   <si>
@@ -270,6 +267,22 @@
   </si>
   <si>
     <t>S-Band Downlink</t>
+  </si>
+  <si>
+    <r>
+      <t>m/s</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -803,66 +816,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -880,6 +833,66 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1184,8 +1197,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1197,24 +1210,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="64" t="s">
+      <c r="A2" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="65" t="s">
+      <c r="B2" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="66">
+      <c r="C2" s="46">
         <v>6378135</v>
       </c>
-      <c r="D2" s="61" t="s">
+      <c r="D2" s="41" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1225,26 +1238,26 @@
       <c r="B3" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="62">
+      <c r="C3" s="42">
         <f>1.38065E-23</f>
         <v>1.38065E-23</v>
       </c>
-      <c r="D3" s="63" t="s">
+      <c r="D3" s="43" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>40</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="62">
-        <v>299790000</v>
-      </c>
-      <c r="D4" s="63" t="s">
-        <v>44</v>
+      <c r="C4" s="42">
+        <v>299792400</v>
+      </c>
+      <c r="D4" s="43" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1254,10 +1267,10 @@
       <c r="B5" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="62">
+      <c r="C5" s="42">
         <v>300000</v>
       </c>
-      <c r="D5" s="60" t="s">
+      <c r="D5" s="40" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1268,12 +1281,12 @@
       <c r="B6" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="62">
+      <c r="C6" s="42">
         <f>100*1000</f>
         <v>100000</v>
       </c>
-      <c r="D6" s="63" t="s">
-        <v>45</v>
+      <c r="D6" s="43" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1283,11 +1296,11 @@
       <c r="B7" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="62">
+      <c r="C7" s="42">
         <v>1000000</v>
       </c>
-      <c r="D7" s="63" t="s">
-        <v>45</v>
+      <c r="D7" s="43" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1297,11 +1310,11 @@
       <c r="B8" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="62">
+      <c r="C8" s="42">
         <v>4000</v>
       </c>
-      <c r="D8" s="63" t="s">
-        <v>45</v>
+      <c r="D8" s="43" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1317,7 +1330,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
@@ -1342,10 +1355,10 @@
       <c r="D1" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="56" t="s">
+      <c r="E1" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="57"/>
+      <c r="F1" s="50"/>
       <c r="G1" s="12"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1355,15 +1368,15 @@
       <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="40">
+      <c r="C2" s="48">
         <v>0.44</v>
       </c>
-      <c r="D2" s="40"/>
+      <c r="D2" s="48"/>
       <c r="E2" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F2" s="33" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G2" s="12"/>
     </row>
@@ -1372,8 +1385,8 @@
         <v>14</v>
       </c>
       <c r="B3" s="3"/>
-      <c r="C3" s="49"/>
-      <c r="D3" s="50"/>
+      <c r="C3" s="54"/>
+      <c r="D3" s="55"/>
       <c r="E3" s="7"/>
       <c r="F3" s="35"/>
       <c r="G3" s="8"/>
@@ -1385,10 +1398,10 @@
       <c r="B4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="40">
+      <c r="C4" s="48">
         <v>100</v>
       </c>
-      <c r="D4" s="40"/>
+      <c r="D4" s="48"/>
       <c r="E4" s="6"/>
       <c r="F4" s="36"/>
     </row>
@@ -1399,10 +1412,10 @@
       <c r="B5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="40">
+      <c r="C5" s="48">
         <v>30</v>
       </c>
-      <c r="D5" s="40"/>
+      <c r="D5" s="48"/>
       <c r="E5" s="7"/>
       <c r="F5" s="22"/>
       <c r="G5" s="12"/>
@@ -1414,10 +1427,10 @@
       <c r="B6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="40">
+      <c r="C6" s="48">
         <v>2</v>
       </c>
-      <c r="D6" s="40"/>
+      <c r="D6" s="48"/>
       <c r="E6" s="7"/>
       <c r="F6" s="8"/>
       <c r="G6" s="12"/>
@@ -1429,11 +1442,11 @@
       <c r="B7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="55">
+      <c r="C7" s="56">
         <f>10*LOG(C4)</f>
         <v>20</v>
       </c>
-      <c r="D7" s="55"/>
+      <c r="D7" s="56"/>
       <c r="E7" s="6"/>
       <c r="F7" s="36"/>
       <c r="G7" s="12"/>
@@ -1445,11 +1458,11 @@
       <c r="B8" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="45">
+      <c r="C8" s="51">
         <f>290*(10^(C6/10)-1)</f>
         <v>169.61902581372294</v>
       </c>
-      <c r="D8" s="45"/>
+      <c r="D8" s="51"/>
       <c r="E8" s="4"/>
       <c r="F8" s="14"/>
       <c r="G8" s="12"/>
@@ -1461,11 +1474,11 @@
       <c r="B9" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="46">
+      <c r="C9" s="61">
         <f>C5-10*LOG(C8)</f>
         <v>7.7052543543729222</v>
       </c>
-      <c r="D9" s="46"/>
+      <c r="D9" s="61"/>
       <c r="E9" s="7"/>
       <c r="F9" s="36"/>
       <c r="G9" s="12"/>
@@ -1515,11 +1528,11 @@
       <c r="B12" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="45">
+      <c r="C12" s="51">
         <f>10*LOG(ul)</f>
         <v>36.020599913279625</v>
       </c>
-      <c r="D12" s="45"/>
+      <c r="D12" s="51"/>
       <c r="E12" s="7"/>
       <c r="F12" s="13"/>
       <c r="G12" s="12"/>
@@ -1531,11 +1544,11 @@
       <c r="B13" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="43">
+      <c r="C13" s="59">
         <f>20*LOG(4*PI()/c_)+10*LOG(k)</f>
-        <v>-376.15130958980478</v>
-      </c>
-      <c r="D13" s="44"/>
+        <v>-376.15137912531861</v>
+      </c>
+      <c r="D13" s="60"/>
       <c r="E13" s="7"/>
       <c r="F13" s="13"/>
       <c r="G13" s="12"/>
@@ -1549,11 +1562,11 @@
       </c>
       <c r="C14" s="31">
         <f>C7+C9-C13-C11-(20*LOG(C2*10^9))-C12</f>
-        <v>69.03750672807098</v>
+        <v>69.03757626358481</v>
       </c>
       <c r="D14" s="31">
         <f>C7+C9-C13-D11-(20*LOG(C2*10^9))-C12</f>
-        <v>85.424485406781059</v>
+        <v>85.42455494229489</v>
       </c>
       <c r="E14" s="7"/>
       <c r="F14" s="8"/>
@@ -1566,15 +1579,15 @@
       <c r="B15" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="53">
+      <c r="C15" s="52">
         <v>0.44</v>
       </c>
-      <c r="D15" s="54"/>
+      <c r="D15" s="53"/>
       <c r="E15" s="37" t="s">
+        <v>46</v>
+      </c>
+      <c r="F15" s="47" t="s">
         <v>47</v>
-      </c>
-      <c r="F15" s="67" t="s">
-        <v>48</v>
       </c>
       <c r="G15" s="12"/>
     </row>
@@ -1583,10 +1596,10 @@
         <v>14</v>
       </c>
       <c r="B16" s="3"/>
-      <c r="C16" s="49" t="s">
+      <c r="C16" s="54" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="50"/>
+      <c r="D16" s="55"/>
       <c r="E16" s="4"/>
       <c r="F16" s="14"/>
     </row>
@@ -1597,13 +1610,13 @@
       <c r="B17" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="49">
+      <c r="C17" s="54">
         <v>5</v>
       </c>
-      <c r="D17" s="50"/>
+      <c r="D17" s="55"/>
       <c r="E17" s="7"/>
       <c r="F17" s="33" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G17" s="12"/>
     </row>
@@ -1614,13 +1627,13 @@
       <c r="B18" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="47">
+      <c r="C18" s="62">
         <v>5</v>
       </c>
-      <c r="D18" s="48"/>
+      <c r="D18" s="63"/>
       <c r="E18" s="7"/>
       <c r="F18" s="35" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K18" s="8"/>
     </row>
@@ -1631,10 +1644,10 @@
       <c r="B19" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="40">
+      <c r="C19" s="48">
         <v>2</v>
       </c>
-      <c r="D19" s="40"/>
+      <c r="D19" s="48"/>
       <c r="E19" s="4"/>
       <c r="F19" s="8"/>
       <c r="G19" s="12"/>
@@ -1646,11 +1659,11 @@
       <c r="B20" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C20" s="51">
+      <c r="C20" s="64">
         <f>10*LOG(C17)</f>
         <v>6.9897000433601884</v>
       </c>
-      <c r="D20" s="52"/>
+      <c r="D20" s="65"/>
       <c r="E20" s="7"/>
       <c r="F20" s="36"/>
       <c r="G20" s="12"/>
@@ -1662,11 +1675,11 @@
       <c r="B21" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C21" s="45">
+      <c r="C21" s="51">
         <f>290*(10^(C19/10)-1)</f>
         <v>169.61902581372294</v>
       </c>
-      <c r="D21" s="45"/>
+      <c r="D21" s="51"/>
       <c r="E21" s="4"/>
       <c r="F21" s="14"/>
       <c r="G21" s="12"/>
@@ -1678,11 +1691,11 @@
       <c r="B22" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="41">
+      <c r="C22" s="57">
         <f>C18-(10*LOG(C21))</f>
         <v>-17.294745645627078</v>
       </c>
-      <c r="D22" s="42"/>
+      <c r="D22" s="58"/>
       <c r="E22" s="6"/>
       <c r="F22" s="36"/>
       <c r="G22" s="12"/>
@@ -1732,14 +1745,14 @@
       <c r="B25" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C25" s="40">
+      <c r="C25" s="48">
         <f>10*LOG(udl)</f>
         <v>50</v>
       </c>
-      <c r="D25" s="40"/>
+      <c r="D25" s="48"/>
       <c r="E25" s="7"/>
       <c r="F25" s="35" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G25" s="12"/>
     </row>
@@ -1750,11 +1763,11 @@
       <c r="B26" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C26" s="43">
+      <c r="C26" s="59">
         <f>20*LOG(4*PI()/c_)+10*LOG(k)</f>
-        <v>-376.15130958980478</v>
-      </c>
-      <c r="D26" s="44"/>
+        <v>-376.15137912531861</v>
+      </c>
+      <c r="D26" s="60"/>
       <c r="E26" s="7"/>
       <c r="F26" s="35"/>
       <c r="G26" s="12"/>
@@ -1768,11 +1781,11 @@
       </c>
       <c r="C27" s="31">
         <f>C20+C22-C26-C24-(20*LOG(C15*10^9))-C25</f>
-        <v>17.047806684710793</v>
+        <v>17.047876220224623</v>
       </c>
       <c r="D27" s="32">
         <f>C20+C22-C26-D24-(20*LOG(C15*10^9))-C25</f>
-        <v>33.434785363420872</v>
+        <v>33.434854898934702</v>
       </c>
       <c r="E27" s="8"/>
       <c r="F27" s="13"/>
@@ -1899,15 +1912,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
     <mergeCell ref="C22:D22"/>
     <mergeCell ref="C25:D25"/>
     <mergeCell ref="C26:D26"/>
@@ -1920,6 +1924,15 @@
     <mergeCell ref="C20:D20"/>
     <mergeCell ref="C21:D21"/>
     <mergeCell ref="C16:D16"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -1955,10 +1968,10 @@
       <c r="D1" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="56" t="s">
+      <c r="E1" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="57"/>
+      <c r="F1" s="50"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
@@ -1967,15 +1980,15 @@
       <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="40">
+      <c r="C2" s="48">
         <v>2.4</v>
       </c>
-      <c r="D2" s="49"/>
+      <c r="D2" s="54"/>
       <c r="E2" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F2" s="33" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G2" s="12"/>
     </row>
@@ -1984,8 +1997,8 @@
         <v>14</v>
       </c>
       <c r="B3" s="3"/>
-      <c r="C3" s="49"/>
-      <c r="D3" s="58"/>
+      <c r="C3" s="54"/>
+      <c r="D3" s="66"/>
       <c r="E3" s="7"/>
       <c r="F3" s="35"/>
       <c r="G3" s="12"/>
@@ -1997,10 +2010,10 @@
       <c r="B4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="40">
+      <c r="C4" s="48">
         <v>100</v>
       </c>
-      <c r="D4" s="40"/>
+      <c r="D4" s="48"/>
       <c r="E4" s="6"/>
       <c r="F4" s="36"/>
     </row>
@@ -2011,10 +2024,10 @@
       <c r="B5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="40">
+      <c r="C5" s="48">
         <v>30</v>
       </c>
-      <c r="D5" s="40"/>
+      <c r="D5" s="48"/>
       <c r="E5" s="7"/>
       <c r="F5" s="35"/>
     </row>
@@ -2025,10 +2038,10 @@
       <c r="B6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="40">
+      <c r="C6" s="48">
         <v>2</v>
       </c>
-      <c r="D6" s="40"/>
+      <c r="D6" s="48"/>
       <c r="E6" s="7"/>
       <c r="F6" s="14"/>
     </row>
@@ -2039,11 +2052,11 @@
       <c r="B7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="55">
+      <c r="C7" s="56">
         <f>10*LOG(C4)</f>
         <v>20</v>
       </c>
-      <c r="D7" s="55"/>
+      <c r="D7" s="56"/>
       <c r="E7" s="6"/>
       <c r="F7" s="36"/>
     </row>
@@ -2054,11 +2067,11 @@
       <c r="B8" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="45">
+      <c r="C8" s="51">
         <f>290*(10^(C6/10)-1)</f>
         <v>169.61902581372294</v>
       </c>
-      <c r="D8" s="45"/>
+      <c r="D8" s="51"/>
       <c r="E8" s="4"/>
       <c r="F8" s="14"/>
     </row>
@@ -2069,11 +2082,11 @@
       <c r="B9" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="46">
+      <c r="C9" s="61">
         <f>C5-10*LOG(C8)</f>
         <v>7.7052543543729222</v>
       </c>
-      <c r="D9" s="46"/>
+      <c r="D9" s="61"/>
       <c r="E9" s="7"/>
       <c r="F9" s="36"/>
     </row>
@@ -2121,11 +2134,11 @@
       <c r="B12" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="45">
+      <c r="C12" s="51">
         <f>10*LOG(ul)</f>
         <v>36.020599913279625</v>
       </c>
-      <c r="D12" s="45"/>
+      <c r="D12" s="51"/>
       <c r="E12" s="7"/>
       <c r="F12" s="13"/>
     </row>
@@ -2136,11 +2149,11 @@
       <c r="B13" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="43">
+      <c r="C13" s="59">
         <f>20*LOG(4*PI()/c_)+10*LOG(k)</f>
-        <v>-376.15130958980478</v>
-      </c>
-      <c r="D13" s="44"/>
+        <v>-376.15137912531861</v>
+      </c>
+      <c r="D13" s="60"/>
       <c r="E13" s="7"/>
       <c r="F13" s="13"/>
     </row>
@@ -2153,11 +2166,11 @@
       </c>
       <c r="C14" s="31">
         <f>C7+C9-C13-C11-(20*LOG(C2*10^9))-C12</f>
-        <v>54.302335423562624</v>
+        <v>54.302404959076455</v>
       </c>
       <c r="D14" s="31">
         <f>C7+C9-C13-D11-(20*LOG(C2*10^9))-C12</f>
-        <v>70.689314102272704</v>
+        <v>70.689383637786534</v>
       </c>
       <c r="E14" s="7"/>
       <c r="F14" s="8"/>
@@ -2171,15 +2184,15 @@
       <c r="B15" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="53">
+      <c r="C15" s="52">
         <v>2.4</v>
       </c>
-      <c r="D15" s="59"/>
+      <c r="D15" s="67"/>
       <c r="E15" s="37" t="s">
-        <v>50</v>
-      </c>
-      <c r="F15" s="67" t="s">
-        <v>48</v>
+        <v>49</v>
+      </c>
+      <c r="F15" s="47" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -2187,10 +2200,10 @@
         <v>14</v>
       </c>
       <c r="B16" s="3"/>
-      <c r="C16" s="49" t="s">
+      <c r="C16" s="54" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="50"/>
+      <c r="D16" s="55"/>
       <c r="E16" s="4"/>
       <c r="F16" s="14"/>
     </row>
@@ -2201,13 +2214,13 @@
       <c r="B17" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="49">
+      <c r="C17" s="54">
         <v>5</v>
       </c>
-      <c r="D17" s="50"/>
+      <c r="D17" s="55"/>
       <c r="E17" s="7"/>
       <c r="F17" s="33" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -2217,13 +2230,13 @@
       <c r="B18" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="47">
+      <c r="C18" s="62">
         <v>5</v>
       </c>
-      <c r="D18" s="48"/>
+      <c r="D18" s="63"/>
       <c r="E18" s="7"/>
       <c r="F18" s="35" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -2233,10 +2246,10 @@
       <c r="B19" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="40">
+      <c r="C19" s="48">
         <v>2</v>
       </c>
-      <c r="D19" s="40"/>
+      <c r="D19" s="48"/>
       <c r="E19" s="4"/>
       <c r="F19" s="8"/>
       <c r="G19" s="12"/>
@@ -2248,11 +2261,11 @@
       <c r="B20" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C20" s="51">
+      <c r="C20" s="64">
         <f>10*LOG(C17)</f>
         <v>6.9897000433601884</v>
       </c>
-      <c r="D20" s="52"/>
+      <c r="D20" s="65"/>
       <c r="E20" s="7"/>
       <c r="F20" s="36"/>
     </row>
@@ -2263,11 +2276,11 @@
       <c r="B21" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C21" s="45">
+      <c r="C21" s="51">
         <f>290*(10^(C19/10)-1)</f>
         <v>169.61902581372294</v>
       </c>
-      <c r="D21" s="45"/>
+      <c r="D21" s="51"/>
       <c r="E21" s="4"/>
       <c r="F21" s="14"/>
     </row>
@@ -2278,11 +2291,11 @@
       <c r="B22" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="41">
+      <c r="C22" s="57">
         <f>C18-(10*LOG(C21))</f>
         <v>-17.294745645627078</v>
       </c>
-      <c r="D22" s="42"/>
+      <c r="D22" s="58"/>
       <c r="E22" s="6"/>
       <c r="F22" s="36"/>
     </row>
@@ -2329,14 +2342,14 @@
       <c r="B25" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C25" s="40">
+      <c r="C25" s="48">
         <f>10*LOG(sdl)</f>
         <v>60</v>
       </c>
-      <c r="D25" s="40"/>
+      <c r="D25" s="48"/>
       <c r="E25" s="7"/>
       <c r="F25" s="35" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2346,11 +2359,11 @@
       <c r="B26" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C26" s="43">
+      <c r="C26" s="59">
         <f>20*LOG(4*PI()/c_)+10*LOG(k)</f>
-        <v>-376.15130958980478</v>
-      </c>
-      <c r="D26" s="44"/>
+        <v>-376.15137912531861</v>
+      </c>
+      <c r="D26" s="60"/>
       <c r="E26" s="7"/>
       <c r="F26" s="35"/>
     </row>
@@ -2363,11 +2376,11 @@
       </c>
       <c r="C27" s="31">
         <f>C20+C22-C26-C24-(20*LOG(C15*10^9))-C25</f>
-        <v>-7.6873646197975631</v>
+        <v>-7.6872950842837326</v>
       </c>
       <c r="D27" s="32">
         <f>C20+C22-C26-D24-(20*LOG(C15*10^9))-C25</f>
-        <v>8.6996140589125162</v>
+        <v>8.6996835944263466</v>
       </c>
       <c r="E27" s="11"/>
       <c r="F27" s="15"/>
@@ -2553,6 +2566,12 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="C25:D25"/>
@@ -2568,12 +2587,6 @@
     <mergeCell ref="C15:D15"/>
     <mergeCell ref="C16:D16"/>
     <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
More precise boltzmann constant
</commit_message>
<xml_diff>
--- a/CMQA/Budgets/RCL-B-COM1.xlsx
+++ b/CMQA/Budgets/RCL-B-COM1.xlsx
@@ -193,64 +193,6 @@
     <t>m</t>
   </si>
   <si>
-    <r>
-      <t>m</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">2 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>kg s</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">-2 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>K</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>-1</t>
-    </r>
-  </si>
-  <si>
     <t>bps</t>
   </si>
   <si>
@@ -283,6 +225,9 @@
       </rPr>
       <t>2</t>
     </r>
+  </si>
+  <si>
+    <t>J/K</t>
   </si>
 </sst>
 </file>
@@ -837,55 +782,55 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1198,7 +1143,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1239,11 +1184,11 @@
         <v>30</v>
       </c>
       <c r="C3" s="42">
-        <f>1.38065E-23</f>
-        <v>1.38065E-23</v>
+        <f>1.380658E-23</f>
+        <v>1.3806580000000001E-23</v>
       </c>
       <c r="D3" s="43" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
@@ -1257,7 +1202,7 @@
         <v>299792400</v>
       </c>
       <c r="D4" s="43" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1286,7 +1231,7 @@
         <v>100000</v>
       </c>
       <c r="D6" s="43" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1300,7 +1245,7 @@
         <v>1000000</v>
       </c>
       <c r="D7" s="43" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1314,7 +1259,7 @@
         <v>4000</v>
       </c>
       <c r="D8" s="43" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -1355,10 +1300,10 @@
       <c r="D1" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="49" t="s">
+      <c r="E1" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="50"/>
+      <c r="F1" s="62"/>
       <c r="G1" s="12"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1373,10 +1318,10 @@
       </c>
       <c r="D2" s="48"/>
       <c r="E2" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F2" s="33" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G2" s="12"/>
     </row>
@@ -1385,8 +1330,8 @@
         <v>14</v>
       </c>
       <c r="B3" s="3"/>
-      <c r="C3" s="54"/>
-      <c r="D3" s="55"/>
+      <c r="C3" s="57"/>
+      <c r="D3" s="58"/>
       <c r="E3" s="7"/>
       <c r="F3" s="35"/>
       <c r="G3" s="8"/>
@@ -1442,11 +1387,11 @@
       <c r="B7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="56">
+      <c r="C7" s="65">
         <f>10*LOG(C4)</f>
         <v>20</v>
       </c>
-      <c r="D7" s="56"/>
+      <c r="D7" s="65"/>
       <c r="E7" s="6"/>
       <c r="F7" s="36"/>
       <c r="G7" s="12"/>
@@ -1458,11 +1403,11 @@
       <c r="B8" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="51">
+      <c r="C8" s="53">
         <f>290*(10^(C6/10)-1)</f>
         <v>169.61902581372294</v>
       </c>
-      <c r="D8" s="51"/>
+      <c r="D8" s="53"/>
       <c r="E8" s="4"/>
       <c r="F8" s="14"/>
       <c r="G8" s="12"/>
@@ -1474,11 +1419,11 @@
       <c r="B9" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="61">
+      <c r="C9" s="54">
         <f>C5-10*LOG(C8)</f>
         <v>7.7052543543729222</v>
       </c>
-      <c r="D9" s="61"/>
+      <c r="D9" s="54"/>
       <c r="E9" s="7"/>
       <c r="F9" s="36"/>
       <c r="G9" s="12"/>
@@ -1528,11 +1473,11 @@
       <c r="B12" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="51">
+      <c r="C12" s="53">
         <f>10*LOG(ul)</f>
         <v>36.020599913279625</v>
       </c>
-      <c r="D12" s="51"/>
+      <c r="D12" s="53"/>
       <c r="E12" s="7"/>
       <c r="F12" s="13"/>
       <c r="G12" s="12"/>
@@ -1544,11 +1489,11 @@
       <c r="B13" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="59">
+      <c r="C13" s="51">
         <f>20*LOG(4*PI()/c_)+10*LOG(k)</f>
-        <v>-376.15137912531861</v>
-      </c>
-      <c r="D13" s="60"/>
+        <v>-376.15135396075277</v>
+      </c>
+      <c r="D13" s="52"/>
       <c r="E13" s="7"/>
       <c r="F13" s="13"/>
       <c r="G13" s="12"/>
@@ -1562,11 +1507,11 @@
       </c>
       <c r="C14" s="31">
         <f>C7+C9-C13-C11-(20*LOG(C2*10^9))-C12</f>
-        <v>69.03757626358481</v>
+        <v>69.03755109901897</v>
       </c>
       <c r="D14" s="31">
         <f>C7+C9-C13-D11-(20*LOG(C2*10^9))-C12</f>
-        <v>85.42455494229489</v>
+        <v>85.424529777729049</v>
       </c>
       <c r="E14" s="7"/>
       <c r="F14" s="8"/>
@@ -1579,15 +1524,15 @@
       <c r="B15" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="52">
+      <c r="C15" s="63">
         <v>0.44</v>
       </c>
-      <c r="D15" s="53"/>
+      <c r="D15" s="64"/>
       <c r="E15" s="37" t="s">
+        <v>45</v>
+      </c>
+      <c r="F15" s="47" t="s">
         <v>46</v>
-      </c>
-      <c r="F15" s="47" t="s">
-        <v>47</v>
       </c>
       <c r="G15" s="12"/>
     </row>
@@ -1596,10 +1541,10 @@
         <v>14</v>
       </c>
       <c r="B16" s="3"/>
-      <c r="C16" s="54" t="s">
+      <c r="C16" s="57" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="55"/>
+      <c r="D16" s="58"/>
       <c r="E16" s="4"/>
       <c r="F16" s="14"/>
     </row>
@@ -1610,13 +1555,13 @@
       <c r="B17" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="54">
+      <c r="C17" s="57">
         <v>5</v>
       </c>
-      <c r="D17" s="55"/>
+      <c r="D17" s="58"/>
       <c r="E17" s="7"/>
       <c r="F17" s="33" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G17" s="12"/>
     </row>
@@ -1627,13 +1572,13 @@
       <c r="B18" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="62">
+      <c r="C18" s="55">
         <v>5</v>
       </c>
-      <c r="D18" s="63"/>
+      <c r="D18" s="56"/>
       <c r="E18" s="7"/>
       <c r="F18" s="35" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K18" s="8"/>
     </row>
@@ -1659,11 +1604,11 @@
       <c r="B20" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C20" s="64">
+      <c r="C20" s="59">
         <f>10*LOG(C17)</f>
         <v>6.9897000433601884</v>
       </c>
-      <c r="D20" s="65"/>
+      <c r="D20" s="60"/>
       <c r="E20" s="7"/>
       <c r="F20" s="36"/>
       <c r="G20" s="12"/>
@@ -1675,11 +1620,11 @@
       <c r="B21" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C21" s="51">
+      <c r="C21" s="53">
         <f>290*(10^(C19/10)-1)</f>
         <v>169.61902581372294</v>
       </c>
-      <c r="D21" s="51"/>
+      <c r="D21" s="53"/>
       <c r="E21" s="4"/>
       <c r="F21" s="14"/>
       <c r="G21" s="12"/>
@@ -1691,11 +1636,11 @@
       <c r="B22" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="57">
+      <c r="C22" s="49">
         <f>C18-(10*LOG(C21))</f>
         <v>-17.294745645627078</v>
       </c>
-      <c r="D22" s="58"/>
+      <c r="D22" s="50"/>
       <c r="E22" s="6"/>
       <c r="F22" s="36"/>
       <c r="G22" s="12"/>
@@ -1752,7 +1697,7 @@
       <c r="D25" s="48"/>
       <c r="E25" s="7"/>
       <c r="F25" s="35" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G25" s="12"/>
     </row>
@@ -1763,11 +1708,11 @@
       <c r="B26" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C26" s="59">
+      <c r="C26" s="51">
         <f>20*LOG(4*PI()/c_)+10*LOG(k)</f>
-        <v>-376.15137912531861</v>
-      </c>
-      <c r="D26" s="60"/>
+        <v>-376.15135396075277</v>
+      </c>
+      <c r="D26" s="52"/>
       <c r="E26" s="7"/>
       <c r="F26" s="35"/>
       <c r="G26" s="12"/>
@@ -1781,11 +1726,11 @@
       </c>
       <c r="C27" s="31">
         <f>C20+C22-C26-C24-(20*LOG(C15*10^9))-C25</f>
-        <v>17.047876220224623</v>
+        <v>17.047851055658782</v>
       </c>
       <c r="D27" s="32">
         <f>C20+C22-C26-D24-(20*LOG(C15*10^9))-C25</f>
-        <v>33.434854898934702</v>
+        <v>33.434829734368861</v>
       </c>
       <c r="E27" s="8"/>
       <c r="F27" s="13"/>
@@ -1912,6 +1857,15 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
     <mergeCell ref="C22:D22"/>
     <mergeCell ref="C25:D25"/>
     <mergeCell ref="C26:D26"/>
@@ -1924,15 +1878,6 @@
     <mergeCell ref="C20:D20"/>
     <mergeCell ref="C21:D21"/>
     <mergeCell ref="C16:D16"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -1968,10 +1913,10 @@
       <c r="D1" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="49" t="s">
+      <c r="E1" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="50"/>
+      <c r="F1" s="62"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
@@ -1983,12 +1928,12 @@
       <c r="C2" s="48">
         <v>2.4</v>
       </c>
-      <c r="D2" s="54"/>
+      <c r="D2" s="57"/>
       <c r="E2" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F2" s="33" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G2" s="12"/>
     </row>
@@ -1997,7 +1942,7 @@
         <v>14</v>
       </c>
       <c r="B3" s="3"/>
-      <c r="C3" s="54"/>
+      <c r="C3" s="57"/>
       <c r="D3" s="66"/>
       <c r="E3" s="7"/>
       <c r="F3" s="35"/>
@@ -2052,11 +1997,11 @@
       <c r="B7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="56">
+      <c r="C7" s="65">
         <f>10*LOG(C4)</f>
         <v>20</v>
       </c>
-      <c r="D7" s="56"/>
+      <c r="D7" s="65"/>
       <c r="E7" s="6"/>
       <c r="F7" s="36"/>
     </row>
@@ -2067,11 +2012,11 @@
       <c r="B8" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="51">
+      <c r="C8" s="53">
         <f>290*(10^(C6/10)-1)</f>
         <v>169.61902581372294</v>
       </c>
-      <c r="D8" s="51"/>
+      <c r="D8" s="53"/>
       <c r="E8" s="4"/>
       <c r="F8" s="14"/>
     </row>
@@ -2082,11 +2027,11 @@
       <c r="B9" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="61">
+      <c r="C9" s="54">
         <f>C5-10*LOG(C8)</f>
         <v>7.7052543543729222</v>
       </c>
-      <c r="D9" s="61"/>
+      <c r="D9" s="54"/>
       <c r="E9" s="7"/>
       <c r="F9" s="36"/>
     </row>
@@ -2134,11 +2079,11 @@
       <c r="B12" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="51">
+      <c r="C12" s="53">
         <f>10*LOG(ul)</f>
         <v>36.020599913279625</v>
       </c>
-      <c r="D12" s="51"/>
+      <c r="D12" s="53"/>
       <c r="E12" s="7"/>
       <c r="F12" s="13"/>
     </row>
@@ -2149,11 +2094,11 @@
       <c r="B13" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="59">
+      <c r="C13" s="51">
         <f>20*LOG(4*PI()/c_)+10*LOG(k)</f>
-        <v>-376.15137912531861</v>
-      </c>
-      <c r="D13" s="60"/>
+        <v>-376.15135396075277</v>
+      </c>
+      <c r="D13" s="52"/>
       <c r="E13" s="7"/>
       <c r="F13" s="13"/>
     </row>
@@ -2166,11 +2111,11 @@
       </c>
       <c r="C14" s="31">
         <f>C7+C9-C13-C11-(20*LOG(C2*10^9))-C12</f>
-        <v>54.302404959076455</v>
+        <v>54.302379794510614</v>
       </c>
       <c r="D14" s="31">
         <f>C7+C9-C13-D11-(20*LOG(C2*10^9))-C12</f>
-        <v>70.689383637786534</v>
+        <v>70.689358473220693</v>
       </c>
       <c r="E14" s="7"/>
       <c r="F14" s="8"/>
@@ -2184,15 +2129,15 @@
       <c r="B15" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="52">
+      <c r="C15" s="63">
         <v>2.4</v>
       </c>
       <c r="D15" s="67"/>
       <c r="E15" s="37" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F15" s="47" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -2200,10 +2145,10 @@
         <v>14</v>
       </c>
       <c r="B16" s="3"/>
-      <c r="C16" s="54" t="s">
+      <c r="C16" s="57" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="55"/>
+      <c r="D16" s="58"/>
       <c r="E16" s="4"/>
       <c r="F16" s="14"/>
     </row>
@@ -2214,13 +2159,13 @@
       <c r="B17" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="54">
+      <c r="C17" s="57">
         <v>5</v>
       </c>
-      <c r="D17" s="55"/>
+      <c r="D17" s="58"/>
       <c r="E17" s="7"/>
       <c r="F17" s="33" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -2230,13 +2175,13 @@
       <c r="B18" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="62">
+      <c r="C18" s="55">
         <v>5</v>
       </c>
-      <c r="D18" s="63"/>
+      <c r="D18" s="56"/>
       <c r="E18" s="7"/>
       <c r="F18" s="35" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -2261,11 +2206,11 @@
       <c r="B20" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C20" s="64">
+      <c r="C20" s="59">
         <f>10*LOG(C17)</f>
         <v>6.9897000433601884</v>
       </c>
-      <c r="D20" s="65"/>
+      <c r="D20" s="60"/>
       <c r="E20" s="7"/>
       <c r="F20" s="36"/>
     </row>
@@ -2276,11 +2221,11 @@
       <c r="B21" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C21" s="51">
+      <c r="C21" s="53">
         <f>290*(10^(C19/10)-1)</f>
         <v>169.61902581372294</v>
       </c>
-      <c r="D21" s="51"/>
+      <c r="D21" s="53"/>
       <c r="E21" s="4"/>
       <c r="F21" s="14"/>
     </row>
@@ -2291,11 +2236,11 @@
       <c r="B22" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="57">
+      <c r="C22" s="49">
         <f>C18-(10*LOG(C21))</f>
         <v>-17.294745645627078</v>
       </c>
-      <c r="D22" s="58"/>
+      <c r="D22" s="50"/>
       <c r="E22" s="6"/>
       <c r="F22" s="36"/>
     </row>
@@ -2349,7 +2294,7 @@
       <c r="D25" s="48"/>
       <c r="E25" s="7"/>
       <c r="F25" s="35" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2359,11 +2304,11 @@
       <c r="B26" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C26" s="59">
+      <c r="C26" s="51">
         <f>20*LOG(4*PI()/c_)+10*LOG(k)</f>
-        <v>-376.15137912531861</v>
-      </c>
-      <c r="D26" s="60"/>
+        <v>-376.15135396075277</v>
+      </c>
+      <c r="D26" s="52"/>
       <c r="E26" s="7"/>
       <c r="F26" s="35"/>
     </row>
@@ -2376,11 +2321,11 @@
       </c>
       <c r="C27" s="31">
         <f>C20+C22-C26-C24-(20*LOG(C15*10^9))-C25</f>
-        <v>-7.6872950842837326</v>
+        <v>-7.6873202488495735</v>
       </c>
       <c r="D27" s="32">
         <f>C20+C22-C26-D24-(20*LOG(C15*10^9))-C25</f>
-        <v>8.6996835944263466</v>
+        <v>8.6996584298605057</v>
       </c>
       <c r="E27" s="11"/>
       <c r="F27" s="15"/>
@@ -2566,12 +2511,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="C25:D25"/>
@@ -2587,6 +2526,12 @@
     <mergeCell ref="C15:D15"/>
     <mergeCell ref="C16:D16"/>
     <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>